<commit_message>
implemented almost all circuits
</commit_message>
<xml_diff>
--- a/lab3/controlunit.xlsx
+++ b/lab3/controlunit.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>Instruction</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -199,6 +199,10 @@
   </si>
   <si>
     <t>instr[15:12]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPR</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -585,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A15" sqref="A15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -603,7 +607,7 @@
     <col min="10" max="10" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -632,10 +636,13 @@
         <v>37</v>
       </c>
       <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -666,8 +673,11 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -698,8 +708,11 @@
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -730,8 +743,11 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -762,8 +778,11 @@
       <c r="J5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -794,8 +813,11 @@
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -826,8 +848,11 @@
       <c r="J7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -858,8 +883,11 @@
       <c r="J8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -890,8 +918,11 @@
       <c r="J9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -919,8 +950,11 @@
       <c r="J10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -948,8 +982,11 @@
       <c r="J11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -977,8 +1014,11 @@
       <c r="J12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1009,8 +1049,11 @@
       <c r="J13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1041,8 +1084,11 @@
       <c r="J14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1070,8 +1116,11 @@
       <c r="J15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1099,8 +1148,11 @@
       <c r="J16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1125,11 +1177,14 @@
       <c r="I17">
         <v>0</v>
       </c>
-      <c r="J17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1154,11 +1209,14 @@
       <c r="I18">
         <v>0</v>
       </c>
-      <c r="J18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1183,11 +1241,14 @@
       <c r="I19">
         <v>0</v>
       </c>
-      <c r="J19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1212,11 +1273,14 @@
       <c r="I20">
         <v>0</v>
       </c>
-      <c r="J20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1244,8 +1308,11 @@
       <c r="J21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1273,8 +1340,11 @@
       <c r="J22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1299,14 +1369,17 @@
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="I23" s="1">
-        <v>1</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1331,14 +1404,17 @@
       <c r="H24">
         <v>0</v>
       </c>
-      <c r="I24" s="1">
-        <v>1</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1369,8 +1445,11 @@
       <c r="J25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1401,8 +1480,11 @@
       <c r="J26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1433,8 +1515,11 @@
       <c r="J27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>43</v>
       </c>

</xml_diff>